<commit_message>
fixed axis min and max
</commit_message>
<xml_diff>
--- a/elevation_power_plot_template.xlsx
+++ b/elevation_power_plot_template.xlsx
@@ -1935,11 +1935,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="228058480"/>
-        <c:axId val="228058872"/>
+        <c:axId val="595620040"/>
+        <c:axId val="595624352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="228058480"/>
+        <c:axId val="595620040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2052,15 +2052,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228058872"/>
+        <c:crossAx val="595624352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="228058872"/>
+        <c:axId val="595624352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="-15"/>
+          <c:min val="-30"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2171,7 +2171,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228058480"/>
+        <c:crossAx val="595620040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2463,11 +2463,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="228055736"/>
-        <c:axId val="228056128"/>
+        <c:axId val="595622000"/>
+        <c:axId val="595620824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="228055736"/>
+        <c:axId val="595622000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2580,12 +2580,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228056128"/>
+        <c:crossAx val="595620824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="228056128"/>
+        <c:axId val="595620824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2698,7 +2698,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228055736"/>
+        <c:crossAx val="595622000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2792,7 +2792,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2912,11 +2911,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="230379864"/>
-        <c:axId val="230376728"/>
+        <c:axId val="596873032"/>
+        <c:axId val="596873816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="230379864"/>
+        <c:axId val="596873032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="90"/>
@@ -2964,7 +2963,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3031,12 +3029,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="230376728"/>
+        <c:crossAx val="596873816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="230376728"/>
+        <c:axId val="596873816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3082,7 +3080,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3149,7 +3146,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="230379864"/>
+        <c:crossAx val="596873032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>

</xml_diff>